<commit_message>
Implemented save to workbook
</commit_message>
<xml_diff>
--- a/Test/2016.116 - A test project folder/Project_Information.xlsx
+++ b/Test/2016.116 - A test project folder/Project_Information.xlsx
@@ -1,31 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10210"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Fast/tim/Documents/code/dev/PSW/Test/2016.116 - A test project folder/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8D0E79C-DBA3-CD46-BC49-ED8058CC394D}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5960" windowWidth="27640" windowHeight="16940" xr2:uid="{62DE40A0-562A-644A-A493-C0AE64AF553F}"/>
+    <workbookView activeTab="0" windowHeight="16940" windowWidth="27640" xWindow="2620" yWindow="480"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="162913" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="38">
   <si>
     <t>Project Information</t>
   </si>
@@ -69,7 +58,7 @@
     <t>Scope</t>
   </si>
   <si>
-    <t>Market ready remodel</t>
+    <t>Market ready remodel of existing floors</t>
   </si>
   <si>
     <t>Description of the project</t>
@@ -84,7 +73,7 @@
     <t>Client Contact Name</t>
   </si>
   <si>
-    <t>Executive</t>
+    <t>Project Executive</t>
   </si>
   <si>
     <t>Job Title</t>
@@ -123,10 +112,19 @@
     <t>Name</t>
   </si>
   <si>
+    <t>Account Manager</t>
+  </si>
+  <si>
+    <t>408 283 0100 x13</t>
+  </si>
+  <si>
+    <t>tim@studiogarchitectsinc.com</t>
+  </si>
+  <si>
     <t>Billing Address</t>
   </si>
   <si>
-    <t>299 Bassett St. #250</t>
+    <t>299 Bassett St. Suite 250</t>
   </si>
   <si>
     <t>San Jose, CA 95110</t>
@@ -135,50 +133,51 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="5">
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color rgb="FF3F3F76"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="12"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <i val="1"/>
+      <color rgb="FF7F7F7F"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
+      <u val="single"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -306,81 +305,72 @@
     </border>
   </borders>
   <cellStyleXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="2" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="2" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="7" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="3" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="1" fillId="2" fontId="4" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="8" fillId="2" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="9" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="2">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
-    <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
-    <cellStyle name="Input" xfId="1" builtinId="20"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="20" name="Input" xfId="1"/>
+    <cellStyle builtinId="53" name="Explanatory Text" xfId="2"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="3"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -680,53 +670,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D769D51-EFF8-8A44-A936-BD23107BD8D1}">
-  <dimension ref="A1:E29"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:E28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E29"/>
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" outlineLevelCol="0"/>
   <cols>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" width="17.1640625"/>
+    <col customWidth="1" max="3" min="3" width="27"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" width="31.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
+    <row r="1" spans="1:5">
+      <c r="A1" s="10" t="n"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="1"/>
-    </row>
-    <row r="2" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
+      <c r="D1" s="3" t="n"/>
+      <c r="E1" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="2" spans="1:5" thickBot="1">
+      <c r="A2" s="10" t="n"/>
+      <c r="B2" s="10" t="n"/>
+      <c r="C2" s="10" t="n"/>
+      <c r="D2" s="3" t="n"/>
+      <c r="E2" s="10" t="n"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="10" t="n"/>
       <c r="B3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="5" t="n">
         <v>2016.116</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1"/>
+      <c r="E3" s="10" t="n"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="10" t="n"/>
       <c r="B4" s="7" t="s">
         <v>4</v>
       </c>
@@ -736,17 +730,17 @@
       <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
+      <c r="E4" s="10" t="n"/>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="10" t="n"/>
+      <c r="B5" s="7" t="n"/>
+      <c r="C5" s="10" t="n"/>
+      <c r="D5" s="9" t="n"/>
+      <c r="E5" s="10" t="n"/>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10" t="n"/>
       <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
@@ -756,17 +750,17 @@
       <c r="D6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+      <c r="E6" s="10" t="n"/>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="10" t="n"/>
+      <c r="D7" s="9" t="n"/>
+      <c r="E7" s="10" t="n"/>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10" t="n"/>
       <c r="B8" s="7" t="s">
         <v>10</v>
       </c>
@@ -776,37 +770,37 @@
       <c r="D8" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:5" ht="49" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="E8" s="10" t="n"/>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="n"/>
+      <c r="B9" s="7" t="n"/>
+      <c r="C9" s="10" t="n"/>
+      <c r="D9" s="9" t="n"/>
+      <c r="E9" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="49" r="10" spans="1:5" thickBot="1">
+      <c r="A10" s="10" t="n"/>
       <c r="B10" s="11" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="13" t="s">
+      <c r="D10" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
+      <c r="E10" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="11" spans="1:5" thickBot="1">
+      <c r="A11" s="10" t="n"/>
+      <c r="B11" s="10" t="n"/>
+      <c r="C11" s="10" t="n"/>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="10" t="n"/>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" s="10" t="n"/>
       <c r="B12" s="4" t="s">
         <v>16</v>
       </c>
@@ -816,50 +810,50 @@
       <c r="D12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="7"/>
+      <c r="E12" s="10" t="n"/>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="10" t="n"/>
+      <c r="B13" s="7" t="n"/>
       <c r="C13" s="8" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="7"/>
+      <c r="E13" s="10" t="n"/>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" s="10" t="n"/>
+      <c r="B14" s="7" t="n"/>
       <c r="C14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="D14" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-      <c r="B15" s="7"/>
+      <c r="E14" s="10" t="n"/>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" s="10" t="n"/>
+      <c r="B15" s="7" t="n"/>
       <c r="C15" s="15" t="s">
         <v>23</v>
       </c>
       <c r="D15" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-      <c r="B16" s="7"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
+      <c r="E15" s="10" t="n"/>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" s="10" t="n"/>
+      <c r="B16" s="7" t="n"/>
+      <c r="C16" s="10" t="n"/>
+      <c r="D16" s="9" t="n"/>
+      <c r="E16" s="10" t="n"/>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="10" t="n"/>
       <c r="B17" s="7" t="s">
         <v>25</v>
       </c>
@@ -869,129 +863,122 @@
       <c r="D17" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1"/>
-      <c r="B18" s="11"/>
+      <c r="E17" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="18" spans="1:5" thickBot="1">
+      <c r="A18" s="10" t="n"/>
+      <c r="B18" s="11" t="n"/>
       <c r="C18" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="D18" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-      <c r="B21" s="4" t="s">
+      <c r="E18" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="19" spans="1:5" thickBot="1">
+      <c r="A19" s="10" t="n"/>
+      <c r="B19" s="10" t="n"/>
+      <c r="C19" s="10" t="n"/>
+      <c r="D19" s="3" t="n"/>
+      <c r="E19" s="10" t="n"/>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="10" t="n"/>
+      <c r="B20" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C20" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D20" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-      <c r="B22" s="7"/>
+      <c r="E20" s="10" t="n"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="10" t="n"/>
+      <c r="B21" s="7" t="n"/>
+      <c r="C21" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="10" t="n"/>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="10" t="n"/>
+      <c r="B22" s="7" t="n"/>
       <c r="C22" s="8" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-      <c r="B23" s="7"/>
-      <c r="C23" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
+      </c>
+      <c r="E22" s="10" t="n"/>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="10" t="n"/>
+      <c r="B23" s="7" t="n"/>
+      <c r="C23" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="D23" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-      <c r="B26" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="D26" s="9" t="s">
+      <c r="E23" s="10" t="n"/>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="10" t="n"/>
+      <c r="B24" s="7" t="n"/>
+      <c r="C24" s="10" t="n"/>
+      <c r="D24" s="9" t="n"/>
+      <c r="E24" s="10" t="n"/>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="10" t="n"/>
+      <c r="B25" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D25" s="9" t="s">
         <v>27</v>
       </c>
-      <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="16" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="17" t="s">
+      <c r="E25" s="10" t="n"/>
+    </row>
+    <row customHeight="1" ht="17" r="26" spans="1:5" thickBot="1">
+      <c r="A26" s="10" t="n"/>
+      <c r="B26" s="11" t="n"/>
+      <c r="C26" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="1"/>
+      <c r="E26" s="10" t="n"/>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" s="10" t="n"/>
+      <c r="B27" s="10" t="n"/>
+      <c r="C27" s="10" t="n"/>
+      <c r="D27" s="3" t="n"/>
+      <c r="E27" s="10" t="n"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="10" t="n"/>
+      <c r="B28" s="10" t="n"/>
+      <c r="C28" s="10" t="n"/>
+      <c r="D28" s="3" t="n"/>
+      <c r="E28" s="10" t="n"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C24" r:id="rId1" xr:uid="{6F8D0CCA-60A1-3340-89B8-689E5DB20ACD}"/>
-    <hyperlink ref="C15" r:id="rId2" xr:uid="{049773DF-5DE0-AC48-BE49-DF8454C229D6}"/>
+    <hyperlink ref="C15" r:id="rId1"/>
+    <hyperlink ref="C23" r:id="rId2"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>